<commit_message>
actualizando separacion de index
</commit_message>
<xml_diff>
--- a/arquitectura/Arquitectura.xlsx
+++ b/arquitectura/Arquitectura.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="8085" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="8085" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Diagrama de Bloques" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Hoja2" sheetId="6" r:id="rId6"/>
     <sheet name="Hoja3" sheetId="7" r:id="rId7"/>
     <sheet name="tabla" sheetId="8" r:id="rId8"/>
+    <sheet name="Hoja1" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
   <si>
     <t>Repórte de Ubicación</t>
   </si>
@@ -252,9 +253,6 @@
     <t>ui</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>ui (descargando)</t>
   </si>
   <si>
@@ -280,6 +278,138 @@
   </si>
   <si>
     <t>RELACION PERSONAS-MAQUINAS (HORARIO INICIO FINAL) INDEXADO POR FECHA HORA</t>
+  </si>
+  <si>
+    <t>VELOCIDAD MAYOR A CERO IGNICION ENCENDIDA</t>
+  </si>
+  <si>
+    <t>usuarios</t>
+  </si>
+  <si>
+    <t>añadir</t>
+  </si>
+  <si>
+    <t>Vidal Alvarez Manuel</t>
+  </si>
+  <si>
+    <t>Wilson Pacco Ramos</t>
+  </si>
+  <si>
+    <t>Juvenal Quiispe</t>
+  </si>
+  <si>
+    <t>Maquinaria</t>
+  </si>
+  <si>
+    <t>tipo maquinaria</t>
+  </si>
+  <si>
+    <t>Operador</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>CAMION 1</t>
+  </si>
+  <si>
+    <t>CAMION 2</t>
+  </si>
+  <si>
+    <t>CAMION 3</t>
+  </si>
+  <si>
+    <t>CAMION 4</t>
+  </si>
+  <si>
+    <t>CAMION 5</t>
+  </si>
+  <si>
+    <t>CACCRAMPA 2</t>
+  </si>
+  <si>
+    <t>CACCRAMPA 1</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>editar</t>
+  </si>
+  <si>
+    <t>eliminar</t>
+  </si>
+  <si>
+    <t>Asignacion de horarios</t>
+  </si>
+  <si>
+    <t>Maquinarias</t>
+  </si>
+  <si>
+    <t>Felix Paupañaupa</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Seleccionar Personal</t>
+  </si>
+  <si>
+    <t>Seleccionar Maquinaria</t>
+  </si>
+  <si>
+    <t>fecha de inicio</t>
+  </si>
+  <si>
+    <t>fecha final</t>
+  </si>
+  <si>
+    <t>guardar</t>
+  </si>
+  <si>
+    <t>calendario y hora</t>
+  </si>
+  <si>
+    <t>Reporte de asiganciones</t>
+  </si>
+  <si>
+    <t>inicio (fecha y hora)</t>
+  </si>
+  <si>
+    <t>final (fecha y hora)</t>
+  </si>
+  <si>
+    <t>Ver reporte</t>
+  </si>
+  <si>
+    <t>Asiganacion (SI/NO)</t>
+  </si>
+  <si>
+    <t>Vidal Alvarez</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Juvenal Quispe</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>mongo db</t>
   </si>
 </sst>
 </file>
@@ -361,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -370,9 +500,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6011,6 +6142,119 @@
           </a:pathLst>
         </a:custGeom>
         <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Flecha abajo 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3867150" y="5943600"/>
+          <a:ext cx="190500" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1438275</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1628775</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Flecha abajo 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="6143625"/>
+          <a:ext cx="190500" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -6365,7 +6609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K1:AE15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="V8" sqref="V8:W15"/>
     </sheetView>
   </sheetViews>
@@ -6520,13 +6764,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
     <col min="2" max="2" width="113.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -6550,53 +6794,53 @@
         <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
         <v>73</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
@@ -6607,10 +6851,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
@@ -6621,10 +6865,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
@@ -6652,9 +6896,9 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E11" t="s">
@@ -6759,18 +7003,18 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
         <v>77</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>37</v>
@@ -6812,9 +7056,9 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>63</v>
       </c>
       <c r="E29" t="s">
@@ -6844,7 +7088,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
         <v>64</v>
@@ -6852,7 +7096,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -7132,4 +7376,387 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:N49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>124</v>
+      </c>
+      <c r="M4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8">
+        <v>42485546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9">
+        <v>2454564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10">
+        <v>4525252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11">
+        <v>4564643215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20">
+        <v>45665465464</v>
+      </c>
+      <c r="D20">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21">
+        <v>45665465464</v>
+      </c>
+      <c r="D21">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22">
+        <v>45665465464</v>
+      </c>
+      <c r="D22">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23">
+        <v>45665465464</v>
+      </c>
+      <c r="D23">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24">
+        <v>45665465464</v>
+      </c>
+      <c r="D24">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>45665465464</v>
+      </c>
+      <c r="D25">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>45665465464</v>
+      </c>
+      <c r="D26">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27">
+        <v>45665465464</v>
+      </c>
+      <c r="D27">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28">
+        <v>45665465464</v>
+      </c>
+      <c r="D28">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
agregando manejo de recursos mineros
</commit_message>
<xml_diff>
--- a/arquitectura/Arquitectura.xlsx
+++ b/arquitectura/Arquitectura.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="124">
   <si>
     <t>Repórte de Ubicación</t>
   </si>
@@ -283,9 +283,6 @@
     <t>VELOCIDAD MAYOR A CERO IGNICION ENCENDIDA</t>
   </si>
   <si>
-    <t>usuarios</t>
-  </si>
-  <si>
     <t>añadir</t>
   </si>
   <si>
@@ -301,18 +298,6 @@
     <t>Maquinaria</t>
   </si>
   <si>
-    <t>tipo maquinaria</t>
-  </si>
-  <si>
-    <t>Operador</t>
-  </si>
-  <si>
-    <t>Telefono</t>
-  </si>
-  <si>
-    <t>GPS</t>
-  </si>
-  <si>
     <t>CAMION 1</t>
   </si>
   <si>
@@ -346,9 +331,6 @@
     <t>Asignacion de horarios</t>
   </si>
   <si>
-    <t>Maquinarias</t>
-  </si>
-  <si>
     <t>Felix Paupañaupa</t>
   </si>
   <si>
@@ -403,13 +385,25 @@
     <t>-</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>mongo db</t>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>Telefono_familia</t>
+  </si>
+  <si>
+    <t>nombre_maquinaria</t>
+  </si>
+  <si>
+    <t>imei</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>Combo box</t>
   </si>
 </sst>
 </file>
@@ -464,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -487,11 +481,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -504,6 +511,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6142,119 +6150,6 @@
           </a:pathLst>
         </a:custGeom>
         <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1428750</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1619250</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Flecha abajo 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3867150" y="5943600"/>
-          <a:ext cx="190500" cy="161925"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1438275</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1628775</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Flecha abajo 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3876675" y="6143625"/>
-          <a:ext cx="190500" cy="161925"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrow">
-          <a:avLst/>
-        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -7380,383 +7275,380 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N49"/>
+  <dimension ref="A5:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="M3" t="s">
+      <c r="D5" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="7">
+        <v>42485546</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2454564</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="7">
+        <v>4525252</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="7">
+        <v>4564643215</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D16" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D17" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D18" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D19" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D20" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D21" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D22" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D23" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="7">
+        <v>45665465464</v>
+      </c>
+      <c r="D24" s="7">
+        <v>958206357</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="N3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L4" t="s">
-        <v>124</v>
-      </c>
-      <c r="M4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C29" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C8">
-        <v>42485546</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9">
-        <v>2454564</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10">
-        <v>4525252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11">
-        <v>4564643215</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="D41" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20">
-        <v>45665465464</v>
-      </c>
-      <c r="D20">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21">
-        <v>45665465464</v>
-      </c>
-      <c r="D21">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22">
-        <v>45665465464</v>
-      </c>
-      <c r="D22">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23">
-        <v>45665465464</v>
-      </c>
-      <c r="D23">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" t="s">
-        <v>97</v>
-      </c>
-      <c r="C24">
-        <v>45665465464</v>
-      </c>
-      <c r="D24">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25">
-        <v>45665465464</v>
-      </c>
-      <c r="D25">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26">
-        <v>45665465464</v>
-      </c>
-      <c r="D26">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27">
-        <v>45665465464</v>
-      </c>
-      <c r="D27">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28">
-        <v>45665465464</v>
-      </c>
-      <c r="D28">
-        <v>958206357</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>109</v>
-      </c>
-      <c r="C34" t="s">
-        <v>112</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="C45" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>